<commit_message>
2nd Question type added along with survey deletion functionality (not working currently)
</commit_message>
<xml_diff>
--- a/SeleniumCDemo/TestDataAccess/TestData.xlsx
+++ b/SeleniumCDemo/TestDataAccess/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ramonma@guilford.edu</t>
   </si>
@@ -45,15 +45,6 @@
     <t>surveyName</t>
   </si>
   <si>
-    <t>What is your name?</t>
-  </si>
-  <si>
-    <t>What is your favorite color?</t>
-  </si>
-  <si>
-    <t>What is the average speed of an unladen swallow?</t>
-  </si>
-  <si>
     <t>Monty Python Questionnaire</t>
   </si>
   <si>
@@ -64,6 +55,21 @@
   </si>
   <si>
     <t>question3</t>
+  </si>
+  <si>
+    <t>singleTextbox|What is your favorite color?</t>
+  </si>
+  <si>
+    <t>singleTextbox|What is the average speed of an unladen swallow?</t>
+  </si>
+  <si>
+    <t>singleTextbox|What is your name?|Male|Female</t>
+  </si>
+  <si>
+    <t>question4</t>
+  </si>
+  <si>
+    <t>checkbox|What is your gender?|Male|Female</t>
   </si>
 </sst>
 </file>
@@ -405,15 +411,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -430,16 +447,19 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -453,16 +473,19 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Dropdown Questions as well as an expanded CSS for the login button
</commit_message>
<xml_diff>
--- a/SeleniumCDemo/TestDataAccess/TestData.xlsx
+++ b/SeleniumCDemo/TestDataAccess/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ramonma@guilford.edu</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>checkbox|What is your gender?|Male|Female</t>
+  </si>
+  <si>
+    <t>question5</t>
+  </si>
+  <si>
+    <t>dropdown|What is your favorite movie?|Anything Monty Python|Something other than Monty Python</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +436,7 @@
     <col min="9" max="9" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -458,8 +464,11 @@
       <c r="I1" t="s">
         <v>16</v>
       </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -486,6 +495,9 @@
       </c>
       <c r="I2" t="s">
         <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized data and refactored a few methods
</commit_message>
<xml_diff>
--- a/SeleniumCDemo/TestDataAccess/TestData.xlsx
+++ b/SeleniumCDemo/TestDataAccess/TestData.xlsx
@@ -69,13 +69,13 @@
     <t>question4</t>
   </si>
   <si>
-    <t>checkbox|What is your gender?|Male|Female</t>
-  </si>
-  <si>
     <t>question5</t>
   </si>
   <si>
-    <t>dropdown|What is your favorite movie?|Anything Monty Python|Something other than Monty Python</t>
+    <t>checkbox|What is your gender?Male|Female</t>
+  </si>
+  <si>
+    <t>dropdown|What is your favorite movie?Anything Monty Python|Something other than Monty Python</t>
   </si>
 </sst>
 </file>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,6 +434,7 @@
     <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="94.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -465,7 +466,7 @@
         <v>16</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -494,7 +495,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>

</xml_diff>